<commit_message>
Update with run of 20 starting with storm 31
</commit_message>
<xml_diff>
--- a/runtime.xlsx
+++ b/runtime.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Runs</t>
   </si>
@@ -42,6 +42,9 @@
   </si>
   <si>
     <t>sdlist</t>
+  </si>
+  <si>
+    <t>sec/run</t>
   </si>
 </sst>
 </file>
@@ -359,15 +362,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -375,13 +381,16 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>10</v>
       </c>
@@ -389,27 +398,64 @@
         <v>820</v>
       </c>
       <c r="C2">
+        <f>B2/A2</f>
+        <v>82</v>
+      </c>
+      <c r="D2">
         <v>5065</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>15</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>5065</v>
       </c>
-      <c r="D3">
-        <v>595836831489578</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>15</v>
+      </c>
+      <c r="B4">
+        <v>1123.7</v>
+      </c>
+      <c r="C4">
+        <f>B4/A4</f>
+        <v>74.913333333333341</v>
+      </c>
+      <c r="D4">
+        <v>1870500046</v>
+      </c>
+      <c r="E4">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>20</v>
+      </c>
+      <c r="C5">
+        <f>B5/A5</f>
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>1448491702</v>
+      </c>
+      <c r="E5">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>